<commit_message>
Copilot ist der einzige Pilot hier
</commit_message>
<xml_diff>
--- a/Gesunde Ernährung/Filter/Antonia_Filter.xlsx
+++ b/Gesunde Ernährung/Filter/Antonia_Filter.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -29,12 +29,60 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="10">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFCCCC"/>
+        <bgColor rgb="00FFCCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFF2CC"/>
+        <bgColor rgb="00FFF2CC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00CCFFCC"/>
+        <bgColor rgb="00CCFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00D9EAD3"/>
+        <bgColor rgb="00D9EAD3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFFF99"/>
+        <bgColor rgb="00FFFF99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00CFE2F3"/>
+        <bgColor rgb="00CFE2F3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFD966"/>
+        <bgColor rgb="00FFD966"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00CCE5FF"/>
+        <bgColor rgb="00CCE5FF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -55,11 +103,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,13 +481,19 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="34" customWidth="1" min="1" max="1"/>
+    <col width="36" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="19" customWidth="1" min="4" max="4"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -458,94 +520,102 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Alkohol</t>
+          <t>Ballaststoffe</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
+          <t>≥30</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
+          <t>g/Tag</t>
+        </is>
+      </c>
+      <c r="D2" s="3" t="inlineStr">
+        <is>
+          <t>Richtwert</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Ballaststoffe</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>≥30</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>g/Tag</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Richtwert</t>
+          <t>Biotin</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>40</v>
+      </c>
+      <c r="C3" s="4" t="inlineStr">
+        <is>
+          <t>µg/Tag</t>
+        </is>
+      </c>
+      <c r="D3" s="5" t="inlineStr">
+        <is>
+          <t>Schätzwert</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Biotin</t>
+          <t>Calcium</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>40</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>µg/Tag</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Schätzwert</t>
+        <v>1000</v>
+      </c>
+      <c r="C4" s="6" t="inlineStr">
+        <is>
+          <t>mg/Tag</t>
+        </is>
+      </c>
+      <c r="D4" s="7" t="inlineStr">
+        <is>
+          <t>Empfohlene Zufuhr</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Calcium</t>
+          <t>Chlorid</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1000</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>mg/Tag</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Empfohlene Zufuhr</t>
+        <v>2300</v>
+      </c>
+      <c r="C5" s="6" t="inlineStr">
+        <is>
+          <t>mg/Tag</t>
+        </is>
+      </c>
+      <c r="D5" s="5" t="inlineStr">
+        <is>
+          <t>Schätzwert</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Chlorid</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>2300</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>mg/Tag</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
+          <t>Chrom</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>30-100</t>
+        </is>
+      </c>
+      <c r="C6" s="4" t="inlineStr">
+        <is>
+          <t>µg/Tag</t>
+        </is>
+      </c>
+      <c r="D6" s="5" t="inlineStr">
         <is>
           <t>Schätzwert</t>
         </is>
@@ -554,80 +624,77 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Chrom</t>
+          <t>Einfach ungesättigte Fettsäuren</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>30-100</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>µg/Tag</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Schätzwert</t>
+          <t>&gt;10</t>
+        </is>
+      </c>
+      <c r="C7" s="8" t="inlineStr">
+        <is>
+          <t>% der Energie</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Einfach ungesättigte Fettsäuren</t>
+          <t>Eisen</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>&gt;10</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>% der Energie</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr"/>
+          <t>Prämenopausal 16 Postmenopausal 14</t>
+        </is>
+      </c>
+      <c r="C8" s="6" t="inlineStr">
+        <is>
+          <t>mg/Tag</t>
+        </is>
+      </c>
+      <c r="D8" s="7" t="inlineStr">
+        <is>
+          <t>Empfohlene Zufuhr</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Eisen</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Prämenopausal 16 Postmenopausal 14</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>mg/Tag</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Empfohlene Zufuhr</t>
+          <t>Energie bei PAL 1,4</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1800</v>
+      </c>
+      <c r="C9" s="9" t="inlineStr">
+        <is>
+          <t>kcal/Tag</t>
+        </is>
+      </c>
+      <c r="D9" s="3" t="inlineStr">
+        <is>
+          <t>Richtwert</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Energie bei PAL 1,4</t>
+          <t>Energie bei PAL 1,6</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1800</v>
-      </c>
-      <c r="C10" t="inlineStr">
+        <v>2100</v>
+      </c>
+      <c r="C10" s="9" t="inlineStr">
         <is>
           <t>kcal/Tag</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="D10" s="3" t="inlineStr">
         <is>
           <t>Richtwert</t>
         </is>
@@ -636,18 +703,18 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Energie bei PAL 1,6</t>
+          <t>Energie bei PAL 1,8</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>2100</v>
-      </c>
-      <c r="C11" t="inlineStr">
+        <v>2400</v>
+      </c>
+      <c r="C11" s="9" t="inlineStr">
         <is>
           <t>kcal/Tag</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="D11" s="3" t="inlineStr">
         <is>
           <t>Richtwert</t>
         </is>
@@ -656,240 +723,240 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Energie bei PAL 1,8</t>
+          <t>EPA_DHA</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>2400</v>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>kcal/Tag</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>Richtwert</t>
+        <v>250</v>
+      </c>
+      <c r="C12" s="6" t="inlineStr">
+        <is>
+          <t>mg/Tag</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>EPA_DHA</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>250</v>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>mg/Tag</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr"/>
+          <t>Fluorid</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>3,0</t>
+        </is>
+      </c>
+      <c r="C13" s="6" t="inlineStr">
+        <is>
+          <t>mg/Tag</t>
+        </is>
+      </c>
+      <c r="D13" s="3" t="inlineStr">
+        <is>
+          <t>Richtwert</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Fluorid</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>3,0</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>mg/Tag</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>Richtwert</t>
+          <t>Folat</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>300</v>
+      </c>
+      <c r="C14" s="4" t="inlineStr">
+        <is>
+          <t>µg/Tag</t>
+        </is>
+      </c>
+      <c r="D14" s="7" t="inlineStr">
+        <is>
+          <t>Empfohlene Zufuhr</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Folat</t>
+          <t>Gesamtfett</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>300</v>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>µg/Tag</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>Empfohlene Zufuhr</t>
+        <v>30</v>
+      </c>
+      <c r="C15" s="8" t="inlineStr">
+        <is>
+          <t>% der Energie</t>
+        </is>
+      </c>
+      <c r="D15" s="3" t="inlineStr">
+        <is>
+          <t>Richtwert</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Gesamtfett</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>30</v>
-      </c>
-      <c r="C16" t="inlineStr">
+          <t>Gesättigte Fettsäuren</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>max. 10</t>
+        </is>
+      </c>
+      <c r="C16" s="8" t="inlineStr">
         <is>
           <t>% der Energie</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>Richtwert</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Gesättigte Fettsäuren</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>max. 10</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>% der Energie</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr"/>
+          <t>Jod</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>200</v>
+      </c>
+      <c r="C17" s="4" t="inlineStr">
+        <is>
+          <t>µg/Tag</t>
+        </is>
+      </c>
+      <c r="D17" s="7" t="inlineStr">
+        <is>
+          <t>Empfohlene Zufuhr</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Jod</t>
+          <t>Kalium</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>200</v>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>µg/Tag</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>Empfohlene Zufuhr</t>
+        <v>4000</v>
+      </c>
+      <c r="C18" s="6" t="inlineStr">
+        <is>
+          <t>mg/Tag</t>
+        </is>
+      </c>
+      <c r="D18" s="5" t="inlineStr">
+        <is>
+          <t>Schätzwert</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Kalium</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>4000</v>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>mg/Tag</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>Schätzwert</t>
+          <t>Kohlenhydrate</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>&gt;50</t>
+        </is>
+      </c>
+      <c r="C19" s="8" t="inlineStr">
+        <is>
+          <t>% der Energie</t>
+        </is>
+      </c>
+      <c r="D19" s="3" t="inlineStr">
+        <is>
+          <t>Richtwert</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Kohlenhydrate</t>
+          <t>Kupfer</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>&gt;50</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>% der Energie</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>Richtwert</t>
+          <t>1,0-1,5</t>
+        </is>
+      </c>
+      <c r="C20" s="6" t="inlineStr">
+        <is>
+          <t>mg/Tag</t>
+        </is>
+      </c>
+      <c r="D20" s="5" t="inlineStr">
+        <is>
+          <t>Schätzwert</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Kupfer</t>
+          <t>Linolsäure</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>1,0-1,5</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>mg/Tag</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>Schätzwert</t>
+          <t>2,5</t>
+        </is>
+      </c>
+      <c r="C21" s="8" t="inlineStr">
+        <is>
+          <t>% der Energie</t>
+        </is>
+      </c>
+      <c r="D21" s="7" t="inlineStr">
+        <is>
+          <t>Empfohlene Zufuhr</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Linolsäure</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>2,5</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>% der Energie</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>Empfohlene Zufuhr</t>
+          <t>Magnesium</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>300</v>
+      </c>
+      <c r="C22" s="6" t="inlineStr">
+        <is>
+          <t>mg/Tag</t>
+        </is>
+      </c>
+      <c r="D22" s="5" t="inlineStr">
+        <is>
+          <t>Schätzwert</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Magnesium</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>300</v>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>mg/Tag</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
+          <t>Mangan</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>2,0-5,0</t>
+        </is>
+      </c>
+      <c r="C23" s="6" t="inlineStr">
+        <is>
+          <t>mg/Tag</t>
+        </is>
+      </c>
+      <c r="D23" s="5" t="inlineStr">
         <is>
           <t>Schätzwert</t>
         </is>
@@ -898,60 +965,57 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Mangan</t>
+          <t>Mehrfach ungesättigte Fettsäuren</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>2,0-5,0</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>mg/Tag</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>Schätzwert</t>
+          <t>7-10</t>
+        </is>
+      </c>
+      <c r="C24" s="8" t="inlineStr">
+        <is>
+          <t>% der Energie</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Mehrfach ungesättigte Fettsäuren</t>
+          <t>Molybdän</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>7-10</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>% der Energie</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr"/>
+          <t>50-100</t>
+        </is>
+      </c>
+      <c r="C25" s="4" t="inlineStr">
+        <is>
+          <t>µg/Tag</t>
+        </is>
+      </c>
+      <c r="D25" s="5" t="inlineStr">
+        <is>
+          <t>Schätzwert</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Molybdän</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>50-100</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>µg/Tag</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
+          <t>Natrium</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>1500</v>
+      </c>
+      <c r="C26" s="6" t="inlineStr">
+        <is>
+          <t>mg/Tag</t>
+        </is>
+      </c>
+      <c r="D26" s="5" t="inlineStr">
         <is>
           <t>Schätzwert</t>
         </is>
@@ -960,58 +1024,58 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Natrium</t>
+          <t>Niacin</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>1500</v>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>mg/Tag</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>Schätzwert</t>
+        <v>12</v>
+      </c>
+      <c r="C27" s="6" t="inlineStr">
+        <is>
+          <t>mg/Tag</t>
+        </is>
+      </c>
+      <c r="D27" s="7" t="inlineStr">
+        <is>
+          <t>Empfohlene Zufuhr</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Niacin</t>
+          <t>Pantothensäure</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>12</v>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>mg/Tag</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>Empfohlene Zufuhr</t>
+        <v>5</v>
+      </c>
+      <c r="C28" s="6" t="inlineStr">
+        <is>
+          <t>mg/Tag</t>
+        </is>
+      </c>
+      <c r="D28" s="5" t="inlineStr">
+        <is>
+          <t>Schätzwert</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Pantothensäure</t>
+          <t>Phosphor</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>5</v>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>mg/Tag</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
+        <v>550</v>
+      </c>
+      <c r="C29" s="6" t="inlineStr">
+        <is>
+          <t>mg/Tag</t>
+        </is>
+      </c>
+      <c r="D29" s="5" t="inlineStr">
         <is>
           <t>Schätzwert</t>
         </is>
@@ -1020,40 +1084,42 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Phosphor</t>
-        </is>
-      </c>
-      <c r="B30" t="n">
-        <v>550</v>
+          <t>Protein</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>0,8</t>
+        </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>mg/Tag</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>Schätzwert</t>
+          <t>g/kg KG/Tag</t>
+        </is>
+      </c>
+      <c r="D30" s="7" t="inlineStr">
+        <is>
+          <t>Empfohlene Zufuhr</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Protein</t>
+          <t>Riboflavin</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>0,8</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>g/kg KG/Tag</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
+          <t>1,1</t>
+        </is>
+      </c>
+      <c r="C31" s="6" t="inlineStr">
+        <is>
+          <t>mg/Tag</t>
+        </is>
+      </c>
+      <c r="D31" s="7" t="inlineStr">
         <is>
           <t>Empfohlene Zufuhr</t>
         </is>
@@ -1062,62 +1128,60 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Riboflavin</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>1,1</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>mg/Tag</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>Empfohlene Zufuhr</t>
+          <t>Selen</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>60</v>
+      </c>
+      <c r="C32" s="4" t="inlineStr">
+        <is>
+          <t>µg/Tag</t>
+        </is>
+      </c>
+      <c r="D32" s="5" t="inlineStr">
+        <is>
+          <t>Schätzwert</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Selen</t>
-        </is>
-      </c>
-      <c r="B33" t="n">
-        <v>60</v>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>µg/Tag</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>Schätzwert</t>
+          <t>Thiamin</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>1,0</t>
+        </is>
+      </c>
+      <c r="C33" s="6" t="inlineStr">
+        <is>
+          <t>mg/Tag</t>
+        </is>
+      </c>
+      <c r="D33" s="7" t="inlineStr">
+        <is>
+          <t>Empfohlene Zufuhr</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Thiamin</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>1,0</t>
-        </is>
+          <t>Vitamin A</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>700</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>mg/Tag</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr">
+          <t>µg-RAE/Tag</t>
+        </is>
+      </c>
+      <c r="D34" s="7" t="inlineStr">
         <is>
           <t>Empfohlene Zufuhr</t>
         </is>
@@ -1126,62 +1190,62 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Vitamin A</t>
-        </is>
-      </c>
-      <c r="B35" t="n">
-        <v>700</v>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>µg-RAE/Tag</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>Empfohlene Zufuhr</t>
+          <t>Vitamin B12 (Cobalamine)</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>4,0</t>
+        </is>
+      </c>
+      <c r="C35" s="4" t="inlineStr">
+        <is>
+          <t>µg/Tag</t>
+        </is>
+      </c>
+      <c r="D35" s="5" t="inlineStr">
+        <is>
+          <t>Schätzwert</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Vitamin B12 (Cobalamine)</t>
+          <t>Vitamin B6</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>4,0</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>µg/Tag</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>Schätzwert</t>
+          <t>1,4</t>
+        </is>
+      </c>
+      <c r="C36" s="6" t="inlineStr">
+        <is>
+          <t>mg/Tag</t>
+        </is>
+      </c>
+      <c r="D36" s="7" t="inlineStr">
+        <is>
+          <t>Empfohlene Zufuhr</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Vitamin B6</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>1,4</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>mg/Tag</t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr">
+          <t>Vitamin C</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>95</v>
+      </c>
+      <c r="C37" s="6" t="inlineStr">
+        <is>
+          <t>mg/Tag</t>
+        </is>
+      </c>
+      <c r="D37" s="7" t="inlineStr">
         <is>
           <t>Empfohlene Zufuhr</t>
         </is>
@@ -1190,38 +1254,38 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Vitamin C</t>
+          <t>Vitamin D</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>95</v>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>mg/Tag</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>Empfohlene Zufuhr</t>
+        <v>20</v>
+      </c>
+      <c r="C38" s="4" t="inlineStr">
+        <is>
+          <t>µg/Tag</t>
+        </is>
+      </c>
+      <c r="D38" s="5" t="inlineStr">
+        <is>
+          <t>Schätzwert</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Vitamin D</t>
+          <t>Vitamin E</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>20</v>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>µg/Tag</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr">
+        <v>12</v>
+      </c>
+      <c r="C39" s="6" t="inlineStr">
+        <is>
+          <t>mg/Tag</t>
+        </is>
+      </c>
+      <c r="D39" s="5" t="inlineStr">
         <is>
           <t>Schätzwert</t>
         </is>
@@ -1230,18 +1294,18 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Vitamin E</t>
+          <t>Vitamin K</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>12</v>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>mg/Tag</t>
-        </is>
-      </c>
-      <c r="D40" t="inlineStr">
+        <v>60</v>
+      </c>
+      <c r="C40" s="4" t="inlineStr">
+        <is>
+          <t>µg/Tag</t>
+        </is>
+      </c>
+      <c r="D40" s="5" t="inlineStr">
         <is>
           <t>Schätzwert</t>
         </is>
@@ -1250,58 +1314,58 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Vitamin K</t>
+          <t>Wasser</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>60</v>
+        <v>1410</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>µg/Tag</t>
-        </is>
-      </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>Schätzwert</t>
+          <t>ml/Tag</t>
+        </is>
+      </c>
+      <c r="D41" s="3" t="inlineStr">
+        <is>
+          <t>Richtwert</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Wasser</t>
+          <t>Zink bei niedriger Phytatzufuhr</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>1410</v>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>ml/Tag</t>
-        </is>
-      </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>Richtwert</t>
+        <v>7</v>
+      </c>
+      <c r="C42" s="6" t="inlineStr">
+        <is>
+          <t>mg/Tag</t>
+        </is>
+      </c>
+      <c r="D42" s="7" t="inlineStr">
+        <is>
+          <t>Empfohlene Zufuhr</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Zink bei niedriger Phytatzufuhr</t>
+          <t>Zink bei hoher Phytatzufuhr</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>7</v>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>mg/Tag</t>
-        </is>
-      </c>
-      <c r="D43" t="inlineStr">
+        <v>10</v>
+      </c>
+      <c r="C43" s="6" t="inlineStr">
+        <is>
+          <t>mg/Tag</t>
+        </is>
+      </c>
+      <c r="D43" s="7" t="inlineStr">
         <is>
           <t>Empfohlene Zufuhr</t>
         </is>
@@ -1310,18 +1374,18 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Zink bei hoher Phytatzufuhr</t>
+          <t>Zink bei mittlerer Phytatzufuhr</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>10</v>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>mg/Tag</t>
-        </is>
-      </c>
-      <c r="D44" t="inlineStr">
+        <v>8</v>
+      </c>
+      <c r="C44" s="6" t="inlineStr">
+        <is>
+          <t>mg/Tag</t>
+        </is>
+      </c>
+      <c r="D44" s="7" t="inlineStr">
         <is>
           <t>Empfohlene Zufuhr</t>
         </is>
@@ -1330,40 +1394,20 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Zink bei mittlerer Phytatzufuhr</t>
-        </is>
-      </c>
-      <c r="B45" t="n">
-        <v>8</v>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>mg/Tag</t>
-        </is>
-      </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>Empfohlene Zufuhr</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
           <t>α-Linolensäure</t>
         </is>
       </c>
-      <c r="B46" t="inlineStr">
+      <c r="B45" t="inlineStr">
         <is>
           <t>0,5</t>
         </is>
       </c>
-      <c r="C46" t="inlineStr">
+      <c r="C45" s="8" t="inlineStr">
         <is>
           <t>% der Energie</t>
         </is>
       </c>
-      <c r="D46" t="inlineStr">
+      <c r="D45" s="5" t="inlineStr">
         <is>
           <t>Schätzwert</t>
         </is>

</xml_diff>